<commit_message>
minor changes to survey csv
</commit_message>
<xml_diff>
--- a/analysis/fullData_analysis/survey_analysis/Thematic Coding.xlsx
+++ b/analysis/fullData_analysis/survey_analysis/Thematic Coding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vasu1\Code\RTmocapFB\analysis\fullData_analysis\survey_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3D3F47-900E-4297-B449-C0C4493F3315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01967D63-7164-48B6-AD18-708E58F7F778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3EB63B0D-FF8A-4255-BBA7-93AAB8B3C41D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{3EB63B0D-FF8A-4255-BBA7-93AAB8B3C41D}"/>
   </bookViews>
   <sheets>
     <sheet name="SW1" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -455,163 +455,151 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -950,26 +938,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{364E062F-9729-432D-B10F-FC73160D932A}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -983,53 +971,53 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="14">
-        <v>2</v>
-      </c>
-      <c r="D3" s="14">
-        <v>1</v>
-      </c>
-      <c r="E3" s="14"/>
+      <c r="C3" s="7">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
-      <c r="B4" s="39" t="s">
+      <c r="A4" s="32"/>
+      <c r="B4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="10">
-        <v>2</v>
-      </c>
-      <c r="D4" s="10">
+      <c r="C4" s="2">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2">
         <v>3</v>
       </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="40" t="s">
+      <c r="A5" s="33"/>
+      <c r="B5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="12">
-        <v>2</v>
-      </c>
-      <c r="D5" s="12">
+      <c r="C5" s="6">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6">
         <v>3</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="2"/>
@@ -1039,8 +1027,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
-      <c r="B7" s="39" t="s">
+      <c r="A7" s="34"/>
+      <c r="B7" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="2">
@@ -1052,8 +1040,8 @@
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="39" t="s">
+      <c r="A8" s="34"/>
+      <c r="B8" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="2">
@@ -1066,53 +1054,53 @@
       <c r="A9" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14">
-        <v>1</v>
-      </c>
-      <c r="E9" s="14"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="36"/>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="10"/>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="36"/>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="10">
-        <v>1</v>
-      </c>
-      <c r="D11" s="10">
-        <v>1</v>
-      </c>
-      <c r="E11" s="10"/>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="57">
+      <c r="B12" s="38"/>
+      <c r="C12" s="28">
         <v>8</v>
       </c>
-      <c r="D12" s="57">
+      <c r="D12" s="28">
         <v>9</v>
       </c>
-      <c r="E12" s="58">
+      <c r="E12" s="29">
         <v>2</v>
       </c>
     </row>
@@ -1125,6 +1113,7 @@
     <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1132,43 +1121,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCDC636-18C8-4603-8145-FB3AC3F58B6A}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="A12:E12"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="32" t="s">
+      <c r="A2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="2">
@@ -1180,8 +1169,8 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="39" t="s">
+      <c r="A4" s="32"/>
+      <c r="B4" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="2">
@@ -1195,8 +1184,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="39" t="s">
+      <c r="A5" s="32"/>
+      <c r="B5" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="2"/>
@@ -1206,36 +1195,36 @@
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="7">
         <v>3</v>
       </c>
-      <c r="D6" s="14">
-        <v>1</v>
-      </c>
-      <c r="E6" s="14"/>
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="34"/>
-      <c r="B7" s="40" t="s">
+      <c r="A7" s="41"/>
+      <c r="B7" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="12">
-        <v>1</v>
-      </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="2">
@@ -1248,58 +1237,58 @@
       <c r="A9" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="14">
-        <v>1</v>
-      </c>
-      <c r="D9" s="14">
-        <v>1</v>
-      </c>
-      <c r="E9" s="14"/>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="36"/>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="10"/>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="36"/>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10">
-        <v>1</v>
-      </c>
-      <c r="E11" s="10"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="55">
+      <c r="B12" s="38"/>
+      <c r="C12" s="26">
         <v>8</v>
       </c>
-      <c r="D12" s="55">
+      <c r="D12" s="26">
         <v>7</v>
       </c>
-      <c r="E12" s="56">
+      <c r="E12" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D13" s="47"/>
+      <c r="D13" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1310,15 +1299,19 @@
     <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6EB92D-6BBF-42CC-9B26-7182144851EF}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1329,287 +1322,287 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="28" t="s">
+      <c r="A2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="10">
-        <v>1</v>
-      </c>
-      <c r="D3" s="10">
-        <v>1</v>
-      </c>
-      <c r="E3" s="10"/>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="39" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="10">
-        <v>1</v>
-      </c>
-      <c r="D4" s="10">
-        <v>1</v>
-      </c>
-      <c r="E4" s="10">
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="39" t="s">
+      <c r="A5" s="45"/>
+      <c r="B5" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="39" t="s">
+      <c r="A6" s="45"/>
+      <c r="B6" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="10">
-        <v>2</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="C6" s="2">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="40" t="s">
+      <c r="A7" s="46"/>
+      <c r="B7" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12">
-        <v>1</v>
-      </c>
-      <c r="E7" s="12">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="14">
-        <v>2</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14">
+      <c r="C8" s="7">
+        <v>2</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="39" t="s">
+      <c r="A9" s="32"/>
+      <c r="B9" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="2">
         <v>4</v>
       </c>
-      <c r="D9" s="10">
-        <v>2</v>
-      </c>
-      <c r="E9" s="10"/>
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="39" t="s">
+      <c r="A10" s="32"/>
+      <c r="B10" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="10">
-        <v>2</v>
-      </c>
-      <c r="D10" s="10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="10"/>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="40" t="s">
+      <c r="A11" s="33"/>
+      <c r="B11" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6">
         <v>4</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="7">
         <v>3</v>
       </c>
-      <c r="D12" s="14">
-        <v>1</v>
-      </c>
-      <c r="E12" s="14"/>
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
-      <c r="B13" s="39" t="s">
+      <c r="A13" s="48"/>
+      <c r="B13" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="10">
-        <v>2</v>
-      </c>
-      <c r="D13" s="10">
-        <v>2</v>
-      </c>
-      <c r="E13" s="10"/>
+      <c r="C13" s="2">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
-      <c r="B14" s="40" t="s">
+      <c r="A14" s="49"/>
+      <c r="B14" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12">
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="23">
-        <v>1</v>
-      </c>
-      <c r="D15" s="23">
+      <c r="C15" s="8">
+        <v>1</v>
+      </c>
+      <c r="D15" s="8">
         <v>3</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="24"/>
-      <c r="B16" s="43" t="s">
+      <c r="A16" s="51"/>
+      <c r="B16" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25">
-        <v>2</v>
-      </c>
-      <c r="E16" s="25"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9">
+        <v>2</v>
+      </c>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="26"/>
-      <c r="B17" s="44" t="s">
+      <c r="A17" s="52"/>
+      <c r="B17" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="27">
-        <v>1</v>
-      </c>
-      <c r="D17" s="27">
-        <v>2</v>
-      </c>
-      <c r="E17" s="27">
+      <c r="C17" s="10">
+        <v>1</v>
+      </c>
+      <c r="D17" s="10">
+        <v>2</v>
+      </c>
+      <c r="E17" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="30">
-        <v>1</v>
-      </c>
-      <c r="D18" s="30">
-        <v>1</v>
-      </c>
-      <c r="E18" s="30">
+      <c r="C18" s="5">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5">
+        <v>1</v>
+      </c>
+      <c r="E18" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="21"/>
-      <c r="B19" s="45" t="s">
+      <c r="A19" s="54"/>
+      <c r="B19" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="31">
-        <v>1</v>
-      </c>
-      <c r="D19" s="31">
-        <v>1</v>
-      </c>
-      <c r="E19" s="31"/>
+      <c r="C19" s="12">
+        <v>1</v>
+      </c>
+      <c r="D19" s="12">
+        <v>1</v>
+      </c>
+      <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="50">
-        <v>2</v>
-      </c>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50">
+      <c r="B20" s="43"/>
+      <c r="C20" s="23">
+        <v>2</v>
+      </c>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="52"/>
-      <c r="C21" s="53">
+      <c r="B21" s="38"/>
+      <c r="C21" s="24">
         <v>12</v>
       </c>
-      <c r="D21" s="53">
+      <c r="D21" s="24">
         <v>12</v>
       </c>
-      <c r="E21" s="54">
+      <c r="E21" s="25">
         <v>12</v>
       </c>
     </row>
@@ -1625,6 +1618,7 @@
     <mergeCell ref="A18:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="85" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1642,13 +1636,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1786,5 +1780,6 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>